<commit_message>
General events added for three months
</commit_message>
<xml_diff>
--- a/Requirements/Milestones.xlsx
+++ b/Requirements/Milestones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a16a53fd2b6f6931/Desktop/EtherInsure/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CC4266D-5D68-41F6-83D6-BE4FCBEE64B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{4CC4266D-5D68-41F6-83D6-BE4FCBEE64B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A25BEA7-6A59-4F74-A915-9EB64862075E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{186D0353-2EF5-489F-BCC2-E521E2BB0A3F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{186D0353-2EF5-489F-BCC2-E521E2BB0A3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Month 1 " sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Milestone 1</t>
   </si>
@@ -210,13 +210,112 @@
   <si>
     <t>Features for Milestone 3:</t>
   </si>
+  <si>
+    <t>General Events throughout the 3 months:</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Weekly Meetings: Schedule weekly meetings with the developer to discuss progress, challenges, and next steps.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GitHub Updates: Regularly push code updates to GitHub to maintain transparency and attract potential customers.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User Testing: Conduct user testing sessions to gather feedback and improve the prototype's usability.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Documentation: Continuously document the development process, codebase, and any important decisions made during the project.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="&quot;• &quot;\ General"/>
+    <numFmt numFmtId="164" formatCode="&quot;• &quot;\ General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -235,12 +334,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -253,6 +346,13 @@
       <family val="1"/>
       <charset val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -278,13 +378,10 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -293,21 +390,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -360,6 +462,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -367,6 +483,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -388,6 +511,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -395,6 +532,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -416,6 +560,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -423,6 +581,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -431,209 +596,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -987,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB247D9-AD85-497E-A061-BA8AFCF2D90A}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1014,17 +976,17 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1051,66 +1013,89 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="28.8">
+      <c r="A15" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="28.8">
+      <c r="A16" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="28.8">
+      <c r="A17" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="28.8">
+      <c r="A18" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C11:C119 B3:B24">
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>UPPER($A1)="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>UPPER($B3)="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>UPPER($B3)="F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B24 C11:C119">
     <cfRule type="expression" priority="5">
       <formula>"'=UPPER($C4)=""F"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C76">
-    <cfRule type="expression" dxfId="47" priority="12">
-      <formula>UPPER($C13)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="13">
-      <formula>UPPER($A11)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="14">
-      <formula>UPPER($C13)="S"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="15">
-      <formula>UPPER($C13)="F"</formula>
+  <conditionalFormatting sqref="B3:B24">
+    <cfRule type="expression" dxfId="24" priority="20">
+      <formula>UPPER($B3)="N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B24">
+    <cfRule type="expression" dxfId="23" priority="21">
+      <formula>UPPER(#REF!)="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="22">
+      <formula>UPPER($B4)="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="23">
+      <formula>UPPER($B4)="F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="expression" dxfId="43" priority="16">
+    <cfRule type="expression" dxfId="20" priority="17">
+      <formula>UPPER(#REF!)="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="18">
+      <formula>UPPER($C11)="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>UPPER($C11)="F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C76">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>UPPER($C11)="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="17">
-      <formula>UPPER(#REF!)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="18">
-      <formula>UPPER($C11)="S"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="19">
-      <formula>UPPER($C11)="F"</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B24">
-    <cfRule type="expression" dxfId="39" priority="20">
-      <formula>UPPER($B4)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="21">
-      <formula>UPPER(#REF!)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="22">
-      <formula>UPPER($B4)="S"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="23">
-      <formula>UPPER($B4)="F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="35" priority="28">
-      <formula>UPPER($B3)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="29">
-      <formula>UPPER($A1)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="30">
-      <formula>UPPER($B3)="S"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="31">
-      <formula>UPPER($B3)="F"</formula>
+  <conditionalFormatting sqref="C13:C76">
+    <cfRule type="expression" dxfId="16" priority="13">
+      <formula>UPPER($A11)="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="14">
+      <formula>UPPER($C13)="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>UPPER($C13)="F"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1121,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC02332-52DF-423E-8A63-6C7038031C65}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1140,7 +1125,7 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1171,7 +1156,7 @@
       <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1195,38 +1180,60 @@
         <v>20</v>
       </c>
     </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="28.8">
+      <c r="A18" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="28.8">
+      <c r="A19" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="28.8">
+      <c r="A20" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="28.8">
+      <c r="A21" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>UPPER($A1)="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>UPPER($B3)="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="9">
+      <formula>UPPER($B3)="F"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3:B17">
     <cfRule type="expression" priority="1">
       <formula>"'=UPPER($C4)=""F"""</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>UPPER($B3)="N"</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B17">
-    <cfRule type="expression" dxfId="15" priority="2">
-      <formula>UPPER($B4)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>UPPER(#REF!)="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>UPPER($B4)="S"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>UPPER($B4)="F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="11" priority="6">
-      <formula>UPPER($B3)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7">
-      <formula>UPPER($A1)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8">
-      <formula>UPPER($B3)="S"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>UPPER($B3)="F"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1236,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1728C87D-3EAD-413C-A7C2-D63BBE1F503F}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1255,7 +1262,7 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1263,22 +1270,22 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1286,7 +1293,7 @@
       <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1311,43 +1318,63 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="28.8">
+      <c r="A15" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="28.8">
+      <c r="A16" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="28.8">
+      <c r="A17" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="28.8">
+      <c r="A18" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>UPPER($A1)="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="8">
+      <formula>UPPER($B3)="S"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>UPPER($B3)="F"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3:B26">
     <cfRule type="expression" priority="1">
       <formula>"'=UPPER($C4)=""F"""</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>UPPER($B3)="N"</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B26">
-    <cfRule type="expression" dxfId="7" priority="2">
-      <formula>UPPER($B4)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>UPPER(#REF!)="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>UPPER($B4)="S"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>UPPER($B4)="F"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>UPPER($B3)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>UPPER($A1)="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>UPPER($B3)="S"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
-      <formula>UPPER($B3)="F"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>